<commit_message>
fix(dashboard): improve weekly absence data calculation
- Fix week calculation logic to handle month transitions correctly
- Add dynamic week count instead of hardcoded 4 weeks
- Implement ISO-8601 compliant week numbering
- Handle edge cases for partial weeks
- Improve date range filtering accuracy

BREAKING CHANGE: getWeekData() now returns actual number of weeks in month
instead of fixed 4 weeks. Dashboard views may need adjustment to handle
variable week counts.
</commit_message>
<xml_diff>
--- a/app/resources/canvas/filiere-canva.xlsx
+++ b/app/resources/canvas/filiere-canva.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ABS-ISTA\app\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ABS-ISTA\app\resources\canvas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2661CC9-5AE5-461F-BAC0-322FE160153F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D135732B-0688-4E55-93A9-6976D372F732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>filiere_name</t>
+    <t>Filiere</t>
   </si>
   <si>
-    <t>secteur_id</t>
+    <t>Secteur</t>
   </si>
 </sst>
 </file>
@@ -81,7 +81,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -92,6 +111,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}" name="Table1" displayName="Table1" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B2" xr:uid="{1AFACD98-3970-4077-8154-94E50ACB833B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{AEC9E63E-4822-4939-BBD3-9EEB4F84567C}" name="Filiere"/>
+    <tableColumn id="2" xr3:uid="{E6BE985D-0B6E-458A-B049-01C68C00C63C}" name="Secteur"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,13 +390,13 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -380,5 +410,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>